<commit_message>
Finished documenting training runs, updated README and results with test info
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="97">
   <si>
     <t xml:space="preserve">Accuracy on Training and Validation</t>
   </si>
@@ -196,6 +196,18 @@
     <t xml:space="preserve">ADDING A POOLING LAYER AFTER 3X3 CONVOLUTION</t>
   </si>
   <si>
+    <t xml:space="preserve">train loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">train acc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test acc</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tiny-C3x16-MP2</t>
   </si>
   <si>
@@ -232,9 +244,18 @@
     <t xml:space="preserve">Huge-1-C3x16-MP2</t>
   </si>
   <si>
+    <t xml:space="preserve">Huge-1-C3x64-MP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* This one is surprisingly slow to train! Actually faster to train this one with 2xconvolutional and pooling layers</t>
+  </si>
+  <si>
     <t xml:space="preserve">Huge-3-C3x16-MP2</t>
   </si>
   <si>
+    <t xml:space="preserve">Huge-3-C3x64-MP2</t>
+  </si>
+  <si>
     <t xml:space="preserve">MULTIPLE CONVOLUTION AND POOLING LAYERS</t>
   </si>
   <si>
@@ -272,6 +293,24 @@
   </si>
   <si>
     <t xml:space="preserve">ADDING DROPOUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large-1-(C3x32-MP2)2+DO(0.2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large-1-(C3x32-MP2)2+DO(0.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huge-1-(C3x16-MP2)2+DO(0.2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huge-1-(C3x16-MP2)2+DO(0.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huge-1-(C3x64-MP2)2+DO(0.2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huge-1-(C3x64-MP2)2+DO(0.5)</t>
   </si>
 </sst>
 </file>
@@ -356,7 +395,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -365,11 +404,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -379,6 +418,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -398,21 +441,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V58"/>
+  <dimension ref="A1:AF63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T66" activeCellId="0" sqref="T66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="13.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="13.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -588,7 +631,7 @@
       <c r="Q4" s="0" t="n">
         <v>0.8862</v>
       </c>
-      <c r="R4" s="0" t="n">
+      <c r="R4" s="4" t="n">
         <f aca="false">(L4+N4+P4)/3</f>
         <v>0.903</v>
       </c>
@@ -658,7 +701,7 @@
       <c r="Q5" s="0" t="n">
         <v>0.1459</v>
       </c>
-      <c r="R5" s="0" t="n">
+      <c r="R5" s="4" t="n">
         <f aca="false">(L5+N5+P5)/3</f>
         <v>0.241066666666667</v>
       </c>
@@ -728,7 +771,7 @@
       <c r="Q6" s="0" t="n">
         <v>0.7244</v>
       </c>
-      <c r="R6" s="0" t="n">
+      <c r="R6" s="4" t="n">
         <f aca="false">(L6+N6+P6)/3</f>
         <v>0.530666666666667</v>
       </c>
@@ -798,7 +841,7 @@
       <c r="Q7" s="0" t="n">
         <v>0.5865</v>
       </c>
-      <c r="R7" s="0" t="n">
+      <c r="R7" s="4" t="n">
         <f aca="false">(L7+N7+P7)/3</f>
         <v>0.520433333333333</v>
       </c>
@@ -865,7 +908,7 @@
       <c r="Q8" s="0" t="n">
         <v>0.8679</v>
       </c>
-      <c r="R8" s="0" t="n">
+      <c r="R8" s="4" t="n">
         <f aca="false">(L8+N8+P8)/3</f>
         <v>0.8584</v>
       </c>
@@ -932,7 +975,7 @@
       <c r="Q9" s="0" t="n">
         <v>0.8853</v>
       </c>
-      <c r="R9" s="0" t="n">
+      <c r="R9" s="4" t="n">
         <f aca="false">(L9+N9+P9)/3</f>
         <v>0.878866666666667</v>
       </c>
@@ -999,7 +1042,7 @@
       <c r="Q10" s="0" t="n">
         <v>0.886</v>
       </c>
-      <c r="R10" s="0" t="n">
+      <c r="R10" s="4" t="n">
         <f aca="false">(L10+N10+P10)/3</f>
         <v>0.882166666666667</v>
       </c>
@@ -1066,7 +1109,7 @@
       <c r="Q11" s="0" t="n">
         <v>0.8847</v>
       </c>
-      <c r="R11" s="0" t="n">
+      <c r="R11" s="4" t="n">
         <f aca="false">(L11+N11+P11)/3</f>
         <v>0.9079</v>
       </c>
@@ -1133,7 +1176,7 @@
       <c r="Q12" s="0" t="n">
         <v>0.8878</v>
       </c>
-      <c r="R12" s="0" t="n">
+      <c r="R12" s="4" t="n">
         <f aca="false">(L12+N12+P12)/3</f>
         <v>0.916133333333333</v>
       </c>
@@ -1200,7 +1243,7 @@
       <c r="Q13" s="0" t="n">
         <v>0.8728</v>
       </c>
-      <c r="R13" s="0" t="n">
+      <c r="R13" s="4" t="n">
         <f aca="false">(L13+N13+P13)/3</f>
         <v>0.909333333333333</v>
       </c>
@@ -1267,7 +1310,7 @@
       <c r="Q14" s="0" t="n">
         <v>0.8849</v>
       </c>
-      <c r="R14" s="0" t="n">
+      <c r="R14" s="4" t="n">
         <f aca="false">(L14+N14+P14)/3</f>
         <v>0.927866666666667</v>
       </c>
@@ -1334,7 +1377,7 @@
       <c r="Q15" s="0" t="n">
         <v>0.9123</v>
       </c>
-      <c r="R15" s="0" t="n">
+      <c r="R15" s="4" t="n">
         <f aca="false">(L15+N15+P15)/3</f>
         <v>0.932233333333333</v>
       </c>
@@ -1401,7 +1444,7 @@
       <c r="Q16" s="0" t="n">
         <v>0.8559</v>
       </c>
-      <c r="R16" s="0" t="n">
+      <c r="R16" s="4" t="n">
         <f aca="false">(L16+N16+P16)/3</f>
         <v>0.9245</v>
       </c>
@@ -1420,6 +1463,7 @@
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="R17" s="4"/>
       <c r="S17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1474,7 +1518,7 @@
       <c r="Q18" s="0" t="n">
         <v>0.956</v>
       </c>
-      <c r="R18" s="0" t="n">
+      <c r="R18" s="4" t="n">
         <f aca="false">(L18+N18+P18)/3</f>
         <v>0.992533333333333</v>
       </c>
@@ -1541,7 +1585,7 @@
       <c r="Q19" s="0" t="n">
         <v>0.9693</v>
       </c>
-      <c r="R19" s="0" t="n">
+      <c r="R19" s="4" t="n">
         <f aca="false">(L19+N19+P19)/3</f>
         <v>0.994133333333333</v>
       </c>
@@ -1608,7 +1652,7 @@
       <c r="Q20" s="0" t="n">
         <v>0.9688</v>
       </c>
-      <c r="R20" s="0" t="n">
+      <c r="R20" s="4" t="n">
         <f aca="false">(L20+N20+P20)/3</f>
         <v>0.993666666666667</v>
       </c>
@@ -1675,7 +1719,7 @@
       <c r="Q21" s="0" t="n">
         <v>0.9657</v>
       </c>
-      <c r="R21" s="0" t="n">
+      <c r="R21" s="4" t="n">
         <f aca="false">(L21+N21+P21)/3</f>
         <v>0.994166666666667</v>
       </c>
@@ -1742,7 +1786,7 @@
       <c r="Q22" s="0" t="n">
         <v>0.965</v>
       </c>
-      <c r="R22" s="0" t="n">
+      <c r="R22" s="4" t="n">
         <f aca="false">(L22+N22+P22)/3</f>
         <v>0.9878</v>
       </c>
@@ -1809,7 +1853,7 @@
       <c r="Q23" s="0" t="n">
         <v>0.1806</v>
       </c>
-      <c r="R23" s="0" t="n">
+      <c r="R23" s="4" t="n">
         <f aca="false">(L23+N23+P23)/3</f>
         <v>0.340333333333333</v>
       </c>
@@ -1876,7 +1920,7 @@
       <c r="Q24" s="0" t="n">
         <v>0.8638</v>
       </c>
-      <c r="R24" s="0" t="n">
+      <c r="R24" s="4" t="n">
         <f aca="false">(L25+N24+P24)/3</f>
         <v>0.6502</v>
       </c>
@@ -1943,7 +1987,7 @@
       <c r="Q25" s="0" t="n">
         <v>0.7282</v>
       </c>
-      <c r="R25" s="0" t="n">
+      <c r="R25" s="4" t="n">
         <f aca="false">(L25+N25+P25)/3</f>
         <v>0.811033333333333</v>
       </c>
@@ -2010,7 +2054,7 @@
       <c r="Q26" s="0" t="n">
         <v>0.9641</v>
       </c>
-      <c r="R26" s="0" t="n">
+      <c r="R26" s="4" t="n">
         <f aca="false">(L26+N26+P26)/3</f>
         <v>0.988666666666667</v>
       </c>
@@ -2077,7 +2121,7 @@
       <c r="Q27" s="0" t="n">
         <v>0.9657</v>
       </c>
-      <c r="R27" s="0" t="n">
+      <c r="R27" s="4" t="n">
         <f aca="false">(L27+N27+P27)/3</f>
         <v>0.989466666666667</v>
       </c>
@@ -2144,7 +2188,7 @@
       <c r="Q28" s="0" t="n">
         <v>0.9588</v>
       </c>
-      <c r="R28" s="0" t="n">
+      <c r="R28" s="4" t="n">
         <f aca="false">(L28+N28+P28)/3</f>
         <v>0.9904</v>
       </c>
@@ -2211,7 +2255,7 @@
       <c r="Q29" s="0" t="n">
         <v>0.9608</v>
       </c>
-      <c r="R29" s="0" t="n">
+      <c r="R29" s="4" t="n">
         <f aca="false">(L29+N29+P29)/3</f>
         <v>0.9921</v>
       </c>
@@ -2278,7 +2322,7 @@
       <c r="Q30" s="0" t="n">
         <v>0.954</v>
       </c>
-      <c r="R30" s="0" t="n">
+      <c r="R30" s="4" t="n">
         <f aca="false">(L30+N30+P30)/3</f>
         <v>0.986133333333333</v>
       </c>
@@ -2297,11 +2341,24 @@
       <c r="A31" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="R31" s="4"/>
       <c r="S31" s="4"/>
+      <c r="V31" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="W31" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="X31" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y31" s="0" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -2316,13 +2373,13 @@
         <v>1</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I32" s="0" t="n">
         <v>0</v>
@@ -2351,7 +2408,7 @@
       <c r="Q32" s="0" t="n">
         <v>0.971</v>
       </c>
-      <c r="R32" s="0" t="n">
+      <c r="R32" s="4" t="n">
         <f aca="false">(L32+N32+P32)/3</f>
         <v>0.990466666666667</v>
       </c>
@@ -2368,7 +2425,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1</v>
@@ -2383,13 +2440,13 @@
         <v>1</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I33" s="0" t="n">
         <v>0</v>
@@ -2418,7 +2475,7 @@
       <c r="Q33" s="0" t="n">
         <v>0.9608</v>
       </c>
-      <c r="R33" s="0" t="n">
+      <c r="R33" s="4" t="n">
         <f aca="false">(L33+N33+P33)/3</f>
         <v>0.9906</v>
       </c>
@@ -2435,7 +2492,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1</v>
@@ -2450,13 +2507,13 @@
         <v>1</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>0</v>
@@ -2485,7 +2542,7 @@
       <c r="Q34" s="0" t="n">
         <v>0.9767</v>
       </c>
-      <c r="R34" s="0" t="n">
+      <c r="R34" s="4" t="n">
         <f aca="false">(L34+N34+P34)/3</f>
         <v>0.994233333333333</v>
       </c>
@@ -2502,7 +2559,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1</v>
@@ -2517,13 +2574,13 @@
         <v>1</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I35" s="0" t="n">
         <v>0</v>
@@ -2552,7 +2609,7 @@
       <c r="Q35" s="0" t="n">
         <v>0.9507</v>
       </c>
-      <c r="R35" s="0" t="n">
+      <c r="R35" s="4" t="n">
         <f aca="false">(L35+N35+P35)/3</f>
         <v>0.978966666666667</v>
       </c>
@@ -2569,7 +2626,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1</v>
@@ -2584,13 +2641,13 @@
         <v>1</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I36" s="0" t="n">
         <v>1</v>
@@ -2619,7 +2676,7 @@
       <c r="Q36" s="0" t="n">
         <v>0.9647</v>
       </c>
-      <c r="R36" s="0" t="n">
+      <c r="R36" s="4" t="n">
         <f aca="false">(L36+N36+P36)/3</f>
         <v>0.9915</v>
       </c>
@@ -2636,7 +2693,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1</v>
@@ -2651,13 +2708,13 @@
         <v>1</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I37" s="0" t="n">
         <v>1</v>
@@ -2686,7 +2743,7 @@
       <c r="Q37" s="0" t="n">
         <v>0.8156</v>
       </c>
-      <c r="R37" s="0" t="n">
+      <c r="R37" s="4" t="n">
         <f aca="false">(L37+N37+P37)/3</f>
         <v>0.726233333333333</v>
       </c>
@@ -2703,7 +2760,7 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1</v>
@@ -2718,13 +2775,13 @@
         <v>1</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I38" s="0" t="n">
         <v>1</v>
@@ -2753,7 +2810,7 @@
       <c r="Q38" s="0" t="n">
         <v>0.9703</v>
       </c>
-      <c r="R38" s="0" t="n">
+      <c r="R38" s="4" t="n">
         <f aca="false">(L38+N38+P38)/3</f>
         <v>0.9902</v>
       </c>
@@ -2770,7 +2827,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1</v>
@@ -2785,13 +2842,13 @@
         <v>1</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I39" s="0" t="n">
         <v>1</v>
@@ -2820,7 +2877,7 @@
       <c r="Q39" s="0" t="n">
         <v>0.9644</v>
       </c>
-      <c r="R39" s="0" t="n">
+      <c r="R39" s="4" t="n">
         <f aca="false">(L39+N39+P39)/3</f>
         <v>0.991533333333333</v>
       </c>
@@ -2837,7 +2894,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1</v>
@@ -2852,13 +2909,13 @@
         <v>1</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I40" s="0" t="n">
         <v>1</v>
@@ -2887,7 +2944,7 @@
       <c r="Q40" s="0" t="n">
         <v>0.9703</v>
       </c>
-      <c r="R40" s="0" t="n">
+      <c r="R40" s="4" t="n">
         <f aca="false">(L40+N40+P40)/3</f>
         <v>0.9936</v>
       </c>
@@ -2902,13 +2959,97 @@
         <v>250</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1"/>
-      <c r="S41" s="4"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="K41" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L41" s="0" t="n">
+        <v>0.9946</v>
+      </c>
+      <c r="M41" s="0" t="n">
+        <v>0.9757</v>
+      </c>
+      <c r="N41" s="0" t="n">
+        <v>0.9882</v>
+      </c>
+      <c r="O41" s="0" t="n">
+        <v>0.9421</v>
+      </c>
+      <c r="P41" s="0" t="n">
+        <v>0.9954</v>
+      </c>
+      <c r="Q41" s="0" t="n">
+        <v>0.9752</v>
+      </c>
+      <c r="R41" s="4" t="n">
+        <f aca="false">(L41+N41+P41)/3</f>
+        <v>0.992733333333333</v>
+      </c>
+      <c r="S41" s="4" t="n">
+        <f aca="false">(M41+O41+Q41)/3</f>
+        <v>0.964333333333333</v>
+      </c>
+      <c r="T41" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="U41" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="V41" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="W41" s="0" t="n">
+        <v>0.1461</v>
+      </c>
+      <c r="X41" s="0" t="n">
+        <v>0.9946</v>
+      </c>
+      <c r="Y41" s="0" t="n">
+        <v>0.9757</v>
+      </c>
+      <c r="Z41" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA41" s="6"/>
+      <c r="AB41" s="6"/>
+      <c r="AC41" s="6"/>
+      <c r="AD41" s="6"/>
+      <c r="AE41" s="6"/>
+      <c r="AF41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1</v>
@@ -2923,13 +3064,13 @@
         <v>1</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I42" s="0" t="n">
         <v>3</v>
@@ -2958,7 +3099,7 @@
       <c r="Q42" s="0" t="n">
         <v>0.9583</v>
       </c>
-      <c r="R42" s="0" t="n">
+      <c r="R42" s="4" t="n">
         <f aca="false">(L42+N42+P42)/3</f>
         <v>0.9907</v>
       </c>
@@ -2972,20 +3113,103 @@
       <c r="U42" s="0" t="n">
         <v>285</v>
       </c>
+      <c r="Z42" s="6"/>
+      <c r="AA42" s="6"/>
+      <c r="AB42" s="6"/>
+      <c r="AC42" s="6"/>
+      <c r="AD42" s="6"/>
+      <c r="AE42" s="6"/>
+      <c r="AF42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1"/>
-      <c r="S43" s="4"/>
+      <c r="A43" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J43" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="K43" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L43" s="0" t="n">
+        <v>0.9923</v>
+      </c>
+      <c r="M43" s="0" t="n">
+        <v>0.969</v>
+      </c>
+      <c r="N43" s="0" t="n">
+        <v>0.9903</v>
+      </c>
+      <c r="O43" s="0" t="n">
+        <v>0.9737</v>
+      </c>
+      <c r="P43" s="0" t="n">
+        <v>0.989</v>
+      </c>
+      <c r="Q43" s="0" t="n">
+        <v>0.9681</v>
+      </c>
+      <c r="R43" s="4" t="n">
+        <f aca="false">(L43+N43+P43)/3</f>
+        <v>0.990533333333334</v>
+      </c>
+      <c r="S43" s="4" t="n">
+        <f aca="false">(M43+O43+Q43)/3</f>
+        <v>0.970266666666667</v>
+      </c>
+      <c r="T43" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="U43" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="V43" s="0" t="n">
+        <v>0.0283</v>
+      </c>
+      <c r="W43" s="0" t="n">
+        <v>0.1347</v>
+      </c>
+      <c r="X43" s="0" t="n">
+        <v>0.9923</v>
+      </c>
+      <c r="Y43" s="0" t="n">
+        <v>0.969</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="R44" s="4"/>
       <c r="S44" s="4"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>2</v>
@@ -3000,13 +3224,13 @@
         <v>2</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I45" s="0" t="n">
         <v>0</v>
@@ -3035,7 +3259,7 @@
       <c r="Q45" s="0" t="n">
         <v>0.9505</v>
       </c>
-      <c r="R45" s="0" t="n">
+      <c r="R45" s="4" t="n">
         <f aca="false">(L45+N45+P45)/3</f>
         <v>0.982133333333333</v>
       </c>
@@ -3052,7 +3276,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>2</v>
@@ -3067,13 +3291,13 @@
         <v>2</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I46" s="0" t="n">
         <v>0</v>
@@ -3102,7 +3326,7 @@
       <c r="Q46" s="0" t="n">
         <v>0.9772</v>
       </c>
-      <c r="R46" s="0" t="n">
+      <c r="R46" s="4" t="n">
         <f aca="false">(L46+N46+P46)/3</f>
         <v>0.989733333333333</v>
       </c>
@@ -3119,7 +3343,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>2</v>
@@ -3134,13 +3358,13 @@
         <v>2</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I47" s="0" t="n">
         <v>0</v>
@@ -3169,7 +3393,7 @@
       <c r="Q47" s="0" t="n">
         <v>0.9859</v>
       </c>
-      <c r="R47" s="0" t="n">
+      <c r="R47" s="4" t="n">
         <f aca="false">(L47+N47+P47)/3</f>
         <v>0.994333333333333</v>
       </c>
@@ -3186,7 +3410,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>2</v>
@@ -3201,13 +3425,13 @@
         <v>2</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I48" s="0" t="n">
         <v>1</v>
@@ -3236,7 +3460,7 @@
       <c r="Q48" s="0" t="n">
         <v>0.9593</v>
       </c>
-      <c r="R48" s="0" t="n">
+      <c r="R48" s="4" t="n">
         <f aca="false">(L48+N48+P48)/3</f>
         <v>0.9873</v>
       </c>
@@ -3253,7 +3477,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>2</v>
@@ -3268,13 +3492,13 @@
         <v>2</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I49" s="0" t="n">
         <v>1</v>
@@ -3303,7 +3527,7 @@
       <c r="Q49" s="0" t="n">
         <v>0.9794</v>
       </c>
-      <c r="R49" s="0" t="n">
+      <c r="R49" s="4" t="n">
         <f aca="false">(L49+N49+P49)/3</f>
         <v>0.989533333333333</v>
       </c>
@@ -3320,13 +3544,74 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="S50" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J50" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="K50" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L50" s="0" t="n">
+        <v>0.9832</v>
+      </c>
+      <c r="M50" s="0" t="n">
+        <v>0.9689</v>
+      </c>
+      <c r="N50" s="0" t="n">
+        <v>0.9833</v>
+      </c>
+      <c r="O50" s="0" t="n">
+        <v>0.9539</v>
+      </c>
+      <c r="P50" s="0" t="n">
+        <v>0.9826</v>
+      </c>
+      <c r="Q50" s="0" t="n">
+        <v>0.9584</v>
+      </c>
+      <c r="R50" s="4" t="n">
+        <f aca="false">(L50+N50+P50)/3</f>
+        <v>0.983033333333333</v>
+      </c>
+      <c r="S50" s="4" t="n">
+        <f aca="false">(M50+O50+Q50)/3</f>
+        <v>0.9604</v>
+      </c>
+      <c r="T50" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="U50" s="0" t="n">
+        <v>230</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>2</v>
@@ -3341,13 +3626,13 @@
         <v>2</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I51" s="0" t="n">
         <v>1</v>
@@ -3376,7 +3661,7 @@
       <c r="Q51" s="0" t="n">
         <v>0.973</v>
       </c>
-      <c r="R51" s="0" t="n">
+      <c r="R51" s="4" t="n">
         <f aca="false">(L51+N51+P51)/3</f>
         <v>0.9932</v>
       </c>
@@ -3393,7 +3678,7 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>2</v>
@@ -3408,13 +3693,13 @@
         <v>2</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I52" s="0" t="n">
         <v>1</v>
@@ -3443,7 +3728,7 @@
       <c r="Q52" s="0" t="n">
         <v>0.9719</v>
       </c>
-      <c r="R52" s="0" t="n">
+      <c r="R52" s="4" t="n">
         <f aca="false">(L52+N52+P52)/3</f>
         <v>0.989033333333333</v>
       </c>
@@ -3460,7 +3745,7 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>2</v>
@@ -3475,13 +3760,13 @@
         <v>2</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I53" s="0" t="n">
         <v>1</v>
@@ -3510,7 +3795,7 @@
       <c r="Q53" s="0" t="n">
         <v>0.9858</v>
       </c>
-      <c r="R53" s="0" t="n">
+      <c r="R53" s="4" t="n">
         <f aca="false">(L53+N53+P53)/3</f>
         <v>0.9977</v>
       </c>
@@ -3524,10 +3809,22 @@
       <c r="U53" s="0" t="n">
         <v>460</v>
       </c>
+      <c r="V53" s="0" t="n">
+        <v>0.0129</v>
+      </c>
+      <c r="W53" s="0" t="n">
+        <v>0.1037</v>
+      </c>
+      <c r="X53" s="0" t="n">
+        <v>0.996</v>
+      </c>
+      <c r="Y53" s="0" t="n">
+        <v>0.9783</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>3</v>
@@ -3542,13 +3839,13 @@
         <v>3</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I54" s="0" t="n">
         <v>1</v>
@@ -3577,7 +3874,7 @@
       <c r="Q54" s="0" t="n">
         <v>0.9801</v>
       </c>
-      <c r="R54" s="0" t="n">
+      <c r="R54" s="4" t="n">
         <f aca="false">(L54+N54+P54)/3</f>
         <v>0.991933333333333</v>
       </c>
@@ -3594,7 +3891,7 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>2</v>
@@ -3609,13 +3906,13 @@
         <v>2</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I55" s="0" t="n">
         <v>3</v>
@@ -3644,7 +3941,7 @@
       <c r="Q55" s="0" t="n">
         <v>0.9808</v>
       </c>
-      <c r="R55" s="0" t="n">
+      <c r="R55" s="4" t="n">
         <f aca="false">(L55+N55+P55)/3</f>
         <v>0.988666666666667</v>
       </c>
@@ -3661,45 +3958,498 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="R56" s="0" t="n">
-        <f aca="false">(L56+N56+P56)/3</f>
-        <v>0</v>
-      </c>
-      <c r="S56" s="4" t="n">
-        <f aca="false">(M56+O56+Q56)/3</f>
-        <v>0</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="R56" s="4"/>
+      <c r="S56" s="4"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R57" s="0" t="n">
+      <c r="A57" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="H57" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I57" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J57" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="K57" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L57" s="0" t="n">
+        <v>0.9787</v>
+      </c>
+      <c r="M57" s="0" t="n">
+        <v>0.9818</v>
+      </c>
+      <c r="N57" s="0" t="n">
+        <v>0.9829</v>
+      </c>
+      <c r="O57" s="0" t="n">
+        <v>0.9843</v>
+      </c>
+      <c r="P57" s="0" t="n">
+        <v>0.9709</v>
+      </c>
+      <c r="Q57" s="0" t="n">
+        <v>0.9808</v>
+      </c>
+      <c r="R57" s="4" t="n">
         <f aca="false">(L57+N57+P57)/3</f>
-        <v>0</v>
+        <v>0.9775</v>
       </c>
       <c r="S57" s="4" t="n">
         <f aca="false">(M57+O57+Q57)/3</f>
-        <v>0</v>
+        <v>0.9823</v>
+      </c>
+      <c r="T57" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="U57" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="V57" s="0" t="n">
+        <v>0.0715</v>
+      </c>
+      <c r="W57" s="0" t="n">
+        <v>0.0744</v>
+      </c>
+      <c r="X57" s="0" t="n">
+        <v>0.9787</v>
+      </c>
+      <c r="Y57" s="0" t="n">
+        <v>0.9818</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R58" s="0" t="n">
+      <c r="A58" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="H58" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J58" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="K58" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L58" s="0" t="n">
+        <v>0.949</v>
+      </c>
+      <c r="M58" s="0" t="n">
+        <v>0.9816</v>
+      </c>
+      <c r="N58" s="0" t="n">
+        <v>0.9284</v>
+      </c>
+      <c r="O58" s="0" t="n">
+        <v>0.9733</v>
+      </c>
+      <c r="P58" s="0" t="n">
+        <v>0.9479</v>
+      </c>
+      <c r="Q58" s="0" t="n">
+        <v>0.9831</v>
+      </c>
+      <c r="R58" s="4" t="n">
         <f aca="false">(L58+N58+P58)/3</f>
-        <v>0</v>
+        <v>0.941766666666667</v>
       </c>
       <c r="S58" s="4" t="n">
         <f aca="false">(M58+O58+Q58)/3</f>
-        <v>0</v>
-      </c>
+        <v>0.979333333333333</v>
+      </c>
+      <c r="T58" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="U58" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="V58" s="0" t="n">
+        <v>0.1611</v>
+      </c>
+      <c r="W58" s="0" t="n">
+        <v>0.0725</v>
+      </c>
+      <c r="X58" s="0" t="n">
+        <v>0.9479</v>
+      </c>
+      <c r="Y58" s="0" t="n">
+        <v>0.9831</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G59" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="H59" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J59" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="K59" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L59" s="0" t="n">
+        <v>0.9877</v>
+      </c>
+      <c r="M59" s="0" t="n">
+        <v>0.9831</v>
+      </c>
+      <c r="N59" s="0" t="n">
+        <v>0.9866</v>
+      </c>
+      <c r="O59" s="0" t="n">
+        <v>0.9814</v>
+      </c>
+      <c r="P59" s="0" t="n">
+        <v>0.9877</v>
+      </c>
+      <c r="Q59" s="0" t="n">
+        <v>0.9565</v>
+      </c>
+      <c r="R59" s="4" t="n">
+        <f aca="false">(L59+N59+P59)/3</f>
+        <v>0.987333333333333</v>
+      </c>
+      <c r="S59" s="4" t="n">
+        <f aca="false">(M59+O59+Q59)/3</f>
+        <v>0.973666666666667</v>
+      </c>
+      <c r="T59" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="U59" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="V59" s="0" t="n">
+        <v>0.0438</v>
+      </c>
+      <c r="W59" s="0" t="n">
+        <v>0.0699</v>
+      </c>
+      <c r="X59" s="0" t="n">
+        <v>0.9877</v>
+      </c>
+      <c r="Y59" s="0" t="n">
+        <v>0.9831</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G60" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="H60" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I60" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J60" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="K60" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L60" s="0" t="n">
+        <v>0.9779</v>
+      </c>
+      <c r="M60" s="0" t="n">
+        <v>0.982</v>
+      </c>
+      <c r="N60" s="0" t="n">
+        <v>0.9714</v>
+      </c>
+      <c r="O60" s="0" t="n">
+        <v>0.9787</v>
+      </c>
+      <c r="P60" s="0" t="n">
+        <v>0.973</v>
+      </c>
+      <c r="Q60" s="0" t="n">
+        <v>0.9813</v>
+      </c>
+      <c r="R60" s="4" t="n">
+        <f aca="false">(L60+N60+P60)/3</f>
+        <v>0.9741</v>
+      </c>
+      <c r="S60" s="4" t="n">
+        <f aca="false">(M60+O60+Q60)/3</f>
+        <v>0.980666666666667</v>
+      </c>
+      <c r="T60" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="U60" s="0" t="n">
+        <v>185</v>
+      </c>
+      <c r="V60" s="0" t="n">
+        <v>0.0742</v>
+      </c>
+      <c r="W60" s="0" t="n">
+        <v>0.0783</v>
+      </c>
+      <c r="X60" s="0" t="n">
+        <v>0.9779</v>
+      </c>
+      <c r="Y60" s="0" t="n">
+        <v>0.982</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G61" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="H61" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I61" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J61" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="K61" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="L61" s="0" t="n">
+        <v>0.9964</v>
+      </c>
+      <c r="M61" s="0" t="n">
+        <v>0.9887</v>
+      </c>
+      <c r="N61" s="0" t="n">
+        <v>0.9932</v>
+      </c>
+      <c r="O61" s="0" t="n">
+        <v>0.9885</v>
+      </c>
+      <c r="P61" s="0" t="n">
+        <v>0.9959</v>
+      </c>
+      <c r="Q61" s="0" t="n">
+        <v>0.9909</v>
+      </c>
+      <c r="R61" s="4" t="n">
+        <f aca="false">(L61+N61+P61)/3</f>
+        <v>0.995166666666667</v>
+      </c>
+      <c r="S61" s="4" t="n">
+        <f aca="false">(M61+O61+Q61)/3</f>
+        <v>0.989366666666667</v>
+      </c>
+      <c r="T61" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="U61" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="V61" s="0" t="n">
+        <v>0.0141</v>
+      </c>
+      <c r="W61" s="0" t="n">
+        <v>0.0555</v>
+      </c>
+      <c r="X61" s="0" t="n">
+        <v>0.9964</v>
+      </c>
+      <c r="Y61" s="0" t="n">
+        <v>0.9887</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G62" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="H62" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J62" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="K62" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L62" s="0" t="n">
+        <v>0.9883</v>
+      </c>
+      <c r="M62" s="0" t="n">
+        <v>0.9919</v>
+      </c>
+      <c r="N62" s="0" t="n">
+        <v>0.9889</v>
+      </c>
+      <c r="O62" s="0" t="n">
+        <v>0.9916</v>
+      </c>
+      <c r="P62" s="0" t="n">
+        <v>0.984</v>
+      </c>
+      <c r="Q62" s="0" t="n">
+        <v>0.9894</v>
+      </c>
+      <c r="R62" s="4" t="n">
+        <f aca="false">(L62+N62+P62)/3</f>
+        <v>0.987066666666667</v>
+      </c>
+      <c r="S62" s="4" t="n">
+        <f aca="false">(M62+O62+Q62)/3</f>
+        <v>0.990966666666667</v>
+      </c>
+      <c r="T62" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="U62" s="0" t="n">
+        <v>450</v>
+      </c>
+      <c r="V62" s="0" t="n">
+        <v>0.0351</v>
+      </c>
+      <c r="W62" s="0" t="n">
+        <v>0.0357</v>
+      </c>
+      <c r="X62" s="0" t="n">
+        <v>0.9883</v>
+      </c>
+      <c r="Y62" s="0" t="n">
+        <v>0.9919</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R63" s="1"/>
+      <c r="S63" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="L1:S1"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="T2:U2"/>
+    <mergeCell ref="Z41:AF42"/>
   </mergeCells>
   <conditionalFormatting sqref="L3:S3">
     <cfRule type="colorScale" priority="2">
@@ -3711,8 +4461,40 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S4:S58">
+  <conditionalFormatting sqref="R63">
     <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF729FCF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S63">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF6D6D"/>
+        <color rgb="FF729FCF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R4:R62">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00CC00"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S4:S62">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Final update to results.xlxs
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -10,17 +10,17 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="98">
   <si>
     <t xml:space="preserve">Accuracy on Training and Validation</t>
   </si>
@@ -308,6 +308,9 @@
   </si>
   <si>
     <t xml:space="preserve">Huge-1-(C3x64-MP2)2+DO(0.2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huge-1-(C3x64-MP2)2+DO(0.4)</t>
   </si>
   <si>
     <t xml:space="preserve">Huge-1-(C3x64-MP2)2+DO(0.5)</t>
@@ -321,13 +324,11 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -346,6 +347,13 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -416,11 +424,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -443,20 +451,11 @@
   </sheetPr>
   <dimension ref="A1:AF63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T66" activeCellId="0" sqref="T66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:Z63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="13.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="13.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.63"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -3175,7 +3174,7 @@
       </c>
       <c r="R43" s="4" t="n">
         <f aca="false">(L43+N43+P43)/3</f>
-        <v>0.990533333333334</v>
+        <v>0.990533333333333</v>
       </c>
       <c r="S43" s="4" t="n">
         <f aca="false">(M43+O43+Q43)/3</f>
@@ -4390,56 +4389,131 @@
         <v>512</v>
       </c>
       <c r="K62" s="0" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L62" s="0" t="n">
-        <v>0.9883</v>
+        <v>0.9891</v>
       </c>
       <c r="M62" s="0" t="n">
-        <v>0.9919</v>
+        <v>0.9854</v>
       </c>
       <c r="N62" s="0" t="n">
-        <v>0.9889</v>
+        <v>0.9902</v>
       </c>
       <c r="O62" s="0" t="n">
-        <v>0.9916</v>
+        <v>0.9907</v>
       </c>
       <c r="P62" s="0" t="n">
-        <v>0.984</v>
+        <v>0.9897</v>
       </c>
       <c r="Q62" s="0" t="n">
-        <v>0.9894</v>
+        <v>0.9909</v>
       </c>
       <c r="R62" s="4" t="n">
         <f aca="false">(L62+N62+P62)/3</f>
-        <v>0.987066666666667</v>
+        <v>0.989666666666667</v>
       </c>
       <c r="S62" s="4" t="n">
         <f aca="false">(M62+O62+Q62)/3</f>
+        <v>0.989</v>
+      </c>
+      <c r="T62" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="U62" s="0" t="n">
+        <v>480</v>
+      </c>
+      <c r="V62" s="0" t="n">
+        <v>0.037</v>
+      </c>
+      <c r="W62" s="0" t="n">
+        <v>0.0665</v>
+      </c>
+      <c r="X62" s="0" t="n">
+        <v>0.9891</v>
+      </c>
+      <c r="Y62" s="0" t="n">
+        <v>0.9854</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="H63" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I63" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J63" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="K63" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L63" s="0" t="n">
+        <v>0.9883</v>
+      </c>
+      <c r="M63" s="0" t="n">
+        <v>0.9919</v>
+      </c>
+      <c r="N63" s="0" t="n">
+        <v>0.9889</v>
+      </c>
+      <c r="O63" s="0" t="n">
+        <v>0.9916</v>
+      </c>
+      <c r="P63" s="0" t="n">
+        <v>0.984</v>
+      </c>
+      <c r="Q63" s="0" t="n">
+        <v>0.9894</v>
+      </c>
+      <c r="R63" s="4" t="n">
+        <f aca="false">(L63+N63+P63)/3</f>
+        <v>0.987066666666667</v>
+      </c>
+      <c r="S63" s="4" t="n">
+        <f aca="false">(M63+O63+Q63)/3</f>
         <v>0.990966666666667</v>
       </c>
-      <c r="T62" s="0" t="n">
+      <c r="T63" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="U62" s="0" t="n">
+      <c r="U63" s="0" t="n">
         <v>450</v>
       </c>
-      <c r="V62" s="0" t="n">
+      <c r="V63" s="0" t="n">
         <v>0.0351</v>
       </c>
-      <c r="W62" s="0" t="n">
+      <c r="W63" s="0" t="n">
         <v>0.0357</v>
       </c>
-      <c r="X62" s="0" t="n">
+      <c r="X63" s="0" t="n">
         <v>0.9883</v>
       </c>
-      <c r="Y62" s="0" t="n">
+      <c r="Y63" s="0" t="n">
         <v>0.9919</v>
       </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R63" s="1"/>
-      <c r="S63" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -4461,43 +4535,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R63">
+  <conditionalFormatting sqref="R4:S63">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFF6D6D"/>
-        <color rgb="FF729FCF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S63">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFF6D6D"/>
-        <color rgb="FF729FCF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R4:R62">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FF00CC00"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S4:S62">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
+        <cfvo type="percentile" val="40"/>
         <cfvo type="max" val="0"/>
         <color rgb="FFFF0000"/>
         <color rgb="FFFFFF00"/>
@@ -4506,11 +4548,11 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>